<commit_message>
Modification is done more features are added
</commit_message>
<xml_diff>
--- a/new_data.xlsx
+++ b/new_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Day_1\d-1\login_page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BFF4E4-CD97-404A-9D47-C0E740B71107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF71DEEB-D3A1-4BF2-95AB-C011C18C123A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -642,7 +642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>

</xml_diff>